<commit_message>
Refactor and complete create task
</commit_message>
<xml_diff>
--- a/Group_Project_CodeSmells.xlsx
+++ b/Group_Project_CodeSmells.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhilyuyen/Documents/git/csci3130/group24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0283BD3C-328F-3B43-B5E8-BC3467FC3767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB2C6C3-9356-0340-BBC6-2441C37C9182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{582FD080-FEA6-42DC-811B-90FB9879C925}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>Code Smell:</t>
   </si>
@@ -137,16 +137,56 @@
   </si>
   <si>
     <t>Decompose the get methods t into various variables.</t>
+  </si>
+  <si>
+    <t>UnableTooAddBoardException</t>
+  </si>
+  <si>
+    <t>It’s an exception which is throws in the workspace service.</t>
+  </si>
+  <si>
+    <t>InvalidWorkspaceIdException</t>
+  </si>
+  <si>
+    <t>InvalidUserIdException</t>
+  </si>
+  <si>
+    <t>It’s an exception which is throws in the workspace and task service.</t>
+  </si>
+  <si>
+    <t>EmptyPasswordException</t>
+  </si>
+  <si>
+    <t>It’s an exception which is throws in the user service.</t>
+  </si>
+  <si>
+    <t>InvalidBoardIdException</t>
+  </si>
+  <si>
+    <t>It’s an exception which is throws in the workspace and board service.</t>
+  </si>
+  <si>
+    <t>InvalidTaskIdException</t>
+  </si>
+  <si>
+    <t>It’s an exception which is throws in the board and task service.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,8 +212,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7DF8F2-A0FC-47DA-8E3F-440C2861F09D}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -499,7 +540,7 @@
     <col min="1" max="1" width="36.1640625" customWidth="1"/>
     <col min="2" max="2" width="42.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="33.1640625" customWidth="1"/>
+    <col min="4" max="4" width="122" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -664,6 +705,90 @@
         <v>33</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add code smells to xlsx
</commit_message>
<xml_diff>
--- a/Group_Project_CodeSmells.xlsx
+++ b/Group_Project_CodeSmells.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhilyuyen/Documents/git/csci3130/group24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB2C6C3-9356-0340-BBC6-2441C37C9182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DAB579-8DB7-3D4D-AE89-B7A0414992E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{582FD080-FEA6-42DC-811B-90FB9879C925}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
   <si>
     <t>Code Smell:</t>
   </si>
@@ -170,6 +170,24 @@
   </si>
   <si>
     <t>It’s an exception which is throws in the board and task service.</t>
+  </si>
+  <si>
+    <t>Magic Number</t>
+  </si>
+  <si>
+    <t>BoardServiceImplTests</t>
+  </si>
+  <si>
+    <t>TaskServiceImplTests</t>
+  </si>
+  <si>
+    <t>Global variables are introduced to replace the magic numbers</t>
+  </si>
+  <si>
+    <t>TaskController</t>
+  </si>
+  <si>
+    <t>Introduce variables to decompose the long statements.</t>
   </si>
 </sst>
 </file>
@@ -529,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7DF8F2-A0FC-47DA-8E3F-440C2861F09D}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -789,6 +807,62 @@
         <v>44</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Replace Group_Project_CodeSmells.xlsx with a new document with updated refactoring and cleaned up a bit.  Good work team.
Tried for a few hours to fix unnecessary abstraction smells, but couldn't find a good way without breaking entire project, so left them as is.
</commit_message>
<xml_diff>
--- a/Group_Project_CodeSmells.xlsx
+++ b/Group_Project_CodeSmells.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhilyuyen/Documents/git/csci3130/group24/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmcki\group24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB2C6C3-9356-0340-BBC6-2441C37C9182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EBC7C2-0227-4D26-98CB-1F0326E09E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{582FD080-FEA6-42DC-811B-90FB9879C925}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{582FD080-FEA6-42DC-811B-90FB9879C925}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
   <si>
     <t>Code Smell:</t>
   </si>
@@ -49,12 +49,6 @@
     <t>Reasoning</t>
   </si>
   <si>
-    <t>Architecture Smell: Scattered Functionality</t>
-  </si>
-  <si>
-    <t>com.group24.trelloclone.user.service</t>
-  </si>
-  <si>
     <t>Deficient Encapsulation</t>
   </si>
   <si>
@@ -79,15 +73,9 @@
     <t>The classes in question are actually utilized in the front end and are there to serve a specific purpose</t>
   </si>
   <si>
-    <t>Implementation Smell: Magic Number</t>
-  </si>
-  <si>
     <t>UserServiceImplTests</t>
   </si>
   <si>
-    <t>These two magic numbers (1L and 2L specifically) are used in testing purposes.  They are used to set up id's for the mock users in order to test specific methods.</t>
-  </si>
-  <si>
     <t>Unnecessary Abstraction</t>
   </si>
   <si>
@@ -118,9 +106,6 @@
     <t>TaskModel</t>
   </si>
   <si>
-    <t>TaskStatusEnum, DatabaseConnectionTests, DashboardApplicationTests, ApplicationConstant</t>
-  </si>
-  <si>
     <t>Unnecessary to refactor</t>
   </si>
   <si>
@@ -170,6 +155,30 @@
   </si>
   <si>
     <t>It’s an exception which is throws in the board and task service.</t>
+  </si>
+  <si>
+    <t>Magic Number</t>
+  </si>
+  <si>
+    <t>BoardServiceImplTests</t>
+  </si>
+  <si>
+    <t>TaskServiceImplTests</t>
+  </si>
+  <si>
+    <t>Global variables are introduced to replace the magic numbers</t>
+  </si>
+  <si>
+    <t>TaskController</t>
+  </si>
+  <si>
+    <t>Introduce variables to decompose the long statements.</t>
+  </si>
+  <si>
+    <t>TaskStatusEnum</t>
+  </si>
+  <si>
+    <t>DatabaseConnectionTests, DashboardApplicationTests</t>
   </si>
 </sst>
 </file>
@@ -529,21 +538,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7DF8F2-A0FC-47DA-8E3F-440C2861F09D}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.1640625" customWidth="1"/>
+    <col min="1" max="1" width="36.109375" customWidth="1"/>
     <col min="2" max="2" width="42.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="122" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -557,236 +566,298 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="1" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="1" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>44</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>